<commit_message>
Working on understanding geico excel data
</commit_message>
<xml_diff>
--- a/GEICO/src/test/java/Utilities/Excel_Data/GeicoExcelData.xlsx
+++ b/GEICO/src/test/java/Utilities/Excel_Data/GeicoExcelData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="9180" windowWidth="28800" windowHeight="8740" tabRatio="500"/>
+    <workbookView xWindow="520" yWindow="4780" windowWidth="28800" windowHeight="8740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="21">
   <si>
     <t>TestCases</t>
   </si>
@@ -84,34 +84,10 @@
     <t>N</t>
   </si>
   <si>
-    <t>dateofbirth</t>
-  </si>
-  <si>
-    <t>Bruce</t>
-  </si>
-  <si>
-    <t>Wayne</t>
-  </si>
-  <si>
-    <t>unitnumber</t>
-  </si>
-  <si>
-    <t>coveragestartdate</t>
-  </si>
-  <si>
     <t>HomeInsuranceStartQuoteByZipcode</t>
   </si>
   <si>
-    <t>901 sout wayne street</t>
-  </si>
-  <si>
-    <t>fake</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>201 south broad street</t>
+    <t>AutoInsuranceStartQuoteByZipcode_PositiveTest</t>
   </si>
 </sst>
 </file>
@@ -466,12 +442,12 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="33.1640625" customWidth="1"/>
+    <col min="1" max="1" width="48.5" customWidth="1"/>
     <col min="5" max="5" width="25.6640625" customWidth="1"/>
     <col min="6" max="6" width="20.33203125" customWidth="1"/>
     <col min="7" max="7" width="18.33203125" customWidth="1"/>
@@ -480,7 +456,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -613,7 +589,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -630,118 +606,48 @@
         <v>5</v>
       </c>
       <c r="E8" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="F8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G8" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="H8" t="s">
-        <v>23</v>
+        <v>9</v>
+      </c>
+      <c r="I8" t="s">
+        <v>10</v>
+      </c>
+      <c r="J8" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>18</v>
       </c>
-      <c r="B9">
-        <v>22044</v>
-      </c>
-      <c r="C9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="1">
-        <v>33159</v>
-      </c>
-      <c r="F9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G9">
-        <v>101</v>
-      </c>
-      <c r="H9" s="1">
-        <v>43355</v>
-      </c>
+      <c r="E9" s="1"/>
+      <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>2</v>
       </c>
-      <c r="B10">
-        <v>20001</v>
-      </c>
-      <c r="C10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10" s="1">
-        <v>31455</v>
-      </c>
-      <c r="F10" t="s">
-        <v>28</v>
-      </c>
-      <c r="G10">
-        <v>909</v>
-      </c>
-      <c r="H10" s="1">
-        <v>43354</v>
-      </c>
+      <c r="E10" s="1"/>
+      <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>18</v>
       </c>
-      <c r="B11">
-        <v>22044</v>
-      </c>
-      <c r="C11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" s="1">
-        <v>33159</v>
-      </c>
-      <c r="F11" t="s">
-        <v>25</v>
-      </c>
-      <c r="G11">
-        <v>101</v>
-      </c>
-      <c r="H11" s="1">
-        <v>43355</v>
-      </c>
+      <c r="E11" s="1"/>
+      <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B12">
-        <v>20001</v>
-      </c>
-      <c r="C12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" t="s">
-        <v>27</v>
-      </c>
-      <c r="E12" s="1">
-        <v>31455</v>
-      </c>
-      <c r="F12" t="s">
-        <v>28</v>
-      </c>
-      <c r="G12">
-        <v>909</v>
-      </c>
-      <c r="H12" s="1">
-        <v>43354</v>
-      </c>
+      <c r="E12" s="1"/>
+      <c r="H12" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>